<commit_message>
modified test cases on overdue fix
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/2351-RBI-EI-DB-DL-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-DLR-LATE-CASH-Makerepayment1.xlsx
+++ b/Mifos Automation Excels/Client/2351-RBI-EI-DB-DL-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-DLR-LATE-CASH-Makerepayment1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" tabRatio="439" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" tabRatio="439" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="9" r:id="rId1"/>
@@ -183,16 +183,16 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -571,14 +571,14 @@
         <v>10000</v>
       </c>
       <c r="B2" s="5">
-        <v>801.94</v>
+        <v>794.27</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5">
         <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>9198.06</v>
+        <v>9205.73</v>
       </c>
       <c r="F2" s="5">
         <v>851.25</v>
@@ -586,10 +586,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>453.94</v>
+        <v>469.94</v>
       </c>
       <c r="B3" s="5">
-        <v>49.31</v>
+        <v>56.98</v>
       </c>
       <c r="C3" s="5">
         <v>0</v>
@@ -598,10 +598,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="5">
-        <v>404.63</v>
+        <v>412.96</v>
       </c>
       <c r="F3" s="5">
-        <v>15.34</v>
+        <v>23.01</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -654,7 +654,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -745,7 +745,7 @@
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
@@ -778,16 +778,16 @@
         <v>851.25</v>
       </c>
       <c r="L3" s="5">
-        <v>835.91</v>
+        <v>828.24</v>
       </c>
       <c r="M3" s="5">
         <v>0</v>
       </c>
       <c r="N3" s="5">
-        <v>835.91</v>
+        <v>828.24</v>
       </c>
       <c r="P3" s="5">
-        <v>15.34</v>
+        <v>23.01</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -811,7 +811,7 @@
         <v>9182.7199999999993</v>
       </c>
       <c r="H4" s="5">
-        <v>15.34</v>
+        <v>23.01</v>
       </c>
       <c r="I4" s="5">
         <v>0</v>
@@ -820,10 +820,10 @@
         <v>0</v>
       </c>
       <c r="K4" s="5">
-        <v>15.34</v>
+        <v>23.01</v>
       </c>
       <c r="L4" s="5">
-        <v>15.34</v>
+        <v>23.01</v>
       </c>
       <c r="M4" s="5">
         <v>0</v>
@@ -848,13 +848,13 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5">
-        <v>835.91</v>
+        <v>828.24</v>
       </c>
       <c r="G5" s="4">
-        <v>8346.81</v>
+        <v>8354.48</v>
       </c>
       <c r="H5" s="5">
-        <v>15.34</v>
+        <v>23.01</v>
       </c>
       <c r="I5" s="5">
         <v>0</v>
@@ -891,13 +891,13 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5">
-        <v>788.75</v>
+        <v>788.7</v>
       </c>
       <c r="G6" s="4">
-        <v>7558.06</v>
+        <v>7565.78</v>
       </c>
       <c r="H6" s="5">
-        <v>62.5</v>
+        <v>62.55</v>
       </c>
       <c r="I6" s="5">
         <v>0</v>
@@ -934,13 +934,13 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5">
-        <v>789.13</v>
+        <v>789.07</v>
       </c>
       <c r="G7" s="4">
-        <v>6768.93</v>
+        <v>6776.71</v>
       </c>
       <c r="H7" s="5">
-        <v>62.12</v>
+        <v>62.18</v>
       </c>
       <c r="I7" s="5">
         <v>0</v>
@@ -977,13 +977,13 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5">
-        <v>793.76</v>
+        <v>793.69</v>
       </c>
       <c r="G8" s="4">
-        <v>5975.17</v>
+        <v>5983.02</v>
       </c>
       <c r="H8" s="5">
-        <v>57.49</v>
+        <v>57.56</v>
       </c>
       <c r="I8" s="5">
         <v>0</v>
@@ -1020,13 +1020,13 @@
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5">
-        <v>802.14</v>
+        <v>802.07</v>
       </c>
       <c r="G9" s="4">
-        <v>5173.03</v>
+        <v>5180.95</v>
       </c>
       <c r="H9" s="5">
-        <v>49.11</v>
+        <v>49.18</v>
       </c>
       <c r="I9" s="5">
         <v>0</v>
@@ -1063,13 +1063,13 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5">
-        <v>807.31</v>
+        <v>807.25</v>
       </c>
       <c r="G10" s="4">
-        <v>4365.72</v>
+        <v>4373.7</v>
       </c>
       <c r="H10" s="5">
-        <v>43.94</v>
+        <v>44</v>
       </c>
       <c r="I10" s="5">
         <v>0</v>
@@ -1106,13 +1106,13 @@
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5">
-        <v>814.17</v>
+        <v>814.1</v>
       </c>
       <c r="G11" s="4">
-        <v>3551.55</v>
+        <v>3559.6</v>
       </c>
       <c r="H11" s="5">
-        <v>37.08</v>
+        <v>37.15</v>
       </c>
       <c r="I11" s="5">
         <v>0</v>
@@ -1149,13 +1149,13 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5">
-        <v>822.06</v>
+        <v>821.99</v>
       </c>
       <c r="G12" s="4">
-        <v>2729.49</v>
+        <v>2737.61</v>
       </c>
       <c r="H12" s="5">
-        <v>29.19</v>
+        <v>29.26</v>
       </c>
       <c r="I12" s="5">
         <v>0</v>
@@ -1192,13 +1192,13 @@
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5">
-        <v>828.07</v>
+        <v>828</v>
       </c>
       <c r="G13" s="4">
-        <v>1901.42</v>
+        <v>1909.61</v>
       </c>
       <c r="H13" s="5">
-        <v>23.18</v>
+        <v>23.25</v>
       </c>
       <c r="I13" s="5">
         <v>0</v>
@@ -1235,13 +1235,13 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5">
-        <v>835.62</v>
+        <v>835.55</v>
       </c>
       <c r="G14" s="4">
-        <v>1065.8</v>
+        <v>1074.06</v>
       </c>
       <c r="H14" s="5">
-        <v>15.63</v>
+        <v>15.7</v>
       </c>
       <c r="I14" s="5">
         <v>0</v>
@@ -1278,13 +1278,13 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="4">
-        <v>1065.8</v>
+        <v>1074.06</v>
       </c>
       <c r="G15" s="5">
         <v>0</v>
       </c>
       <c r="H15" s="5">
-        <v>9.0500000000000007</v>
+        <v>9.1199999999999992</v>
       </c>
       <c r="I15" s="5">
         <v>0</v>
@@ -1293,7 +1293,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="4">
-        <v>1074.8499999999999</v>
+        <v>1083.18</v>
       </c>
       <c r="L15" s="5">
         <v>0</v>
@@ -1305,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="P15" s="4">
-        <v>1074.8499999999999</v>
+        <v>1083.18</v>
       </c>
     </row>
   </sheetData>
@@ -1315,26 +1315,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>28</v>
       </c>
@@ -1366,9 +1367,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
-        <v>185</v>
+        <v>3</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>30</v>
@@ -1383,10 +1384,10 @@
         <v>851.25</v>
       </c>
       <c r="F2" s="10">
-        <v>801.94</v>
+        <v>794.27</v>
       </c>
       <c r="G2" s="10">
-        <v>49.31</v>
+        <v>56.98</v>
       </c>
       <c r="H2" s="10">
         <v>0</v>
@@ -1395,12 +1396,14 @@
         <v>0</v>
       </c>
       <c r="J2" s="12">
-        <v>9198.06</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>9205.73</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>30</v>

</xml_diff>